<commit_message>
Next step for June 2022
Ppt slides and final next steps
</commit_message>
<xml_diff>
--- a/EDA/site_cluster_class.xlsx
+++ b/EDA/site_cluster_class.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\mchang\repos\WHONDRS\WHONDRS_collab\WHONDRS_collaboration\EDA\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{919DD1BC-3781-47F0-A22C-3CC5EC4B7C88}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{04D5D484-5F27-4B24-9FF9-36AC1D064541}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="38400" windowHeight="17730" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="38400" windowHeight="17730" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Top_CF_Cluster_Class" sheetId="2" r:id="rId1"/>
@@ -26,7 +26,7 @@
   <pivotCaches>
     <pivotCache cacheId="0" r:id="rId4"/>
     <pivotCache cacheId="1" r:id="rId5"/>
-    <pivotCache cacheId="15" r:id="rId6"/>
+    <pivotCache cacheId="2" r:id="rId6"/>
   </pivotCaches>
 </workbook>
 </file>
@@ -2361,7 +2361,7 @@
     <xf numFmtId="0" fontId="1" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="10">
+  <cellXfs count="11">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="1" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="33" borderId="0" xfId="0" applyFill="1"/>
@@ -2374,6 +2374,7 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="16" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="9" fontId="16" fillId="0" borderId="0" xfId="1" applyFont="1"/>
   </cellXfs>
   <cellStyles count="43">
     <cellStyle name="20% - Accent1" xfId="20" builtinId="30" customBuiltin="1"/>
@@ -2447,7 +2448,7 @@
     </mc:Fallback>
   </mc:AlternateContent>
   <c:pivotSource>
-    <c:name>[water_site_cluster_class.xlsx]Top_CF_Cluster_Class!PivotTable8</c:name>
+    <c:name>[site_cluster_class.xlsx]Top_CF_Cluster_Class!PivotTable8</c:name>
     <c:fmtId val="0"/>
   </c:pivotSource>
   <c:chart>
@@ -3265,7 +3266,7 @@
     </mc:Fallback>
   </mc:AlternateContent>
   <c:pivotSource>
-    <c:name>[water_site_cluster_class.xlsx]site_cluster_class!PivotTable9</c:name>
+    <c:name>[site_cluster_class.xlsx]site_cluster_class!PivotTable9</c:name>
     <c:fmtId val="0"/>
   </c:pivotSource>
   <c:chart>
@@ -4684,7 +4685,7 @@
     </mc:Fallback>
   </mc:AlternateContent>
   <c:pivotSource>
-    <c:name>[water_site_cluster_class.xlsx]sed_site_class!PivotTable6</c:name>
+    <c:name>[site_cluster_class.xlsx]sed_site_class!PivotTable6</c:name>
     <c:fmtId val="0"/>
   </c:pivotSource>
   <c:chart>
@@ -6803,15 +6804,15 @@
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
       <xdr:col>3</xdr:col>
-      <xdr:colOff>254000</xdr:colOff>
+      <xdr:colOff>400050</xdr:colOff>
       <xdr:row>17</xdr:row>
-      <xdr:rowOff>120650</xdr:rowOff>
+      <xdr:rowOff>88900</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>17</xdr:col>
-      <xdr:colOff>318567</xdr:colOff>
+      <xdr:colOff>464617</xdr:colOff>
       <xdr:row>60</xdr:row>
-      <xdr:rowOff>131526</xdr:rowOff>
+      <xdr:rowOff>99776</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -6834,7 +6835,7 @@
       </xdr:blipFill>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="2730500" y="3251200"/>
+          <a:off x="2876550" y="3219450"/>
           <a:ext cx="8840267" cy="7929326"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
@@ -15074,7 +15075,7 @@
     <dataField name="Average of %Other" fld="17" subtotal="average" baseField="0" baseItem="3"/>
   </dataFields>
   <conditionalFormats count="3">
-    <conditionalFormat priority="3">
+    <conditionalFormat priority="2">
       <pivotAreas count="1">
         <pivotArea type="data" collapsedLevelsAreSubtotals="1" fieldPosition="0">
           <references count="2">
@@ -15089,13 +15090,13 @@
               <x v="8"/>
             </reference>
             <reference field="1" count="1">
-              <x v="0"/>
+              <x v="2"/>
             </reference>
           </references>
         </pivotArea>
       </pivotAreas>
     </conditionalFormat>
-    <conditionalFormat priority="2">
+    <conditionalFormat priority="3">
       <pivotAreas count="1">
         <pivotArea type="data" collapsedLevelsAreSubtotals="1" fieldPosition="0">
           <references count="2">
@@ -15116,7 +15117,7 @@
         </pivotArea>
       </pivotAreas>
     </conditionalFormat>
-    <conditionalFormat priority="1">
+    <conditionalFormat priority="4">
       <pivotAreas count="1">
         <pivotArea type="data" collapsedLevelsAreSubtotals="1" fieldPosition="0">
           <references count="2">
@@ -15131,7 +15132,7 @@
               <x v="8"/>
             </reference>
             <reference field="1" count="1">
-              <x v="2"/>
+              <x v="0"/>
             </reference>
           </references>
         </pivotArea>
@@ -15270,7 +15271,7 @@
 </file>
 
 <file path=xl/pivotTables/pivotTable3.xml><?xml version="1.0" encoding="utf-8"?>
-<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{E4974917-1FE9-42DF-82AF-DE6DDFF12A99}" name="PivotTable6" cacheId="15" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="6" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="6" indent="0" outline="1" outlineData="1" multipleFieldFilters="0" chartFormat="1">
+<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{E4974917-1FE9-42DF-82AF-DE6DDFF12A99}" name="PivotTable6" cacheId="2" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="6" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="6" indent="0" outline="1" outlineData="1" multipleFieldFilters="0" chartFormat="1">
   <location ref="Y2:Z5" firstHeaderRow="1" firstDataRow="1" firstDataCol="1"/>
   <pivotFields count="1">
     <pivotField axis="axisRow" dataField="1" showAll="0">
@@ -15623,8 +15624,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:J63"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A2" sqref="A2"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="T1" sqref="T1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -16527,10 +16528,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
-  <dimension ref="A1:AG266"/>
+  <dimension ref="A1:AG267"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="Z5" sqref="Z5"/>
+      <selection activeCell="B2" sqref="B2:C263"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -37710,6 +37711,84 @@
         <v>1.0000000000000002</v>
       </c>
     </row>
+    <row r="267" spans="1:22" x14ac:dyDescent="0.35">
+      <c r="C267">
+        <f>SUM(C2:C266)</f>
+        <v>20349</v>
+      </c>
+      <c r="D267">
+        <f t="shared" ref="D267:L267" si="55">SUM(D2:D266)</f>
+        <v>7934</v>
+      </c>
+      <c r="E267">
+        <f t="shared" si="55"/>
+        <v>80238</v>
+      </c>
+      <c r="F267">
+        <f t="shared" si="55"/>
+        <v>394877</v>
+      </c>
+      <c r="G267">
+        <f t="shared" si="55"/>
+        <v>13463</v>
+      </c>
+      <c r="H267">
+        <f t="shared" si="55"/>
+        <v>3086</v>
+      </c>
+      <c r="I267">
+        <f t="shared" si="55"/>
+        <v>69398</v>
+      </c>
+      <c r="J267">
+        <f t="shared" si="55"/>
+        <v>97402</v>
+      </c>
+      <c r="K267">
+        <f t="shared" si="55"/>
+        <v>5995</v>
+      </c>
+      <c r="L267">
+        <f t="shared" si="55"/>
+        <v>692742</v>
+      </c>
+      <c r="M267" s="1">
+        <f>C267/$L$267</f>
+        <v>2.9374572351611422E-2</v>
+      </c>
+      <c r="N267" s="1">
+        <f t="shared" ref="N267:U267" si="56">D267/$L$267</f>
+        <v>1.1453037350124578E-2</v>
+      </c>
+      <c r="O267" s="1">
+        <f t="shared" si="56"/>
+        <v>0.11582667140147414</v>
+      </c>
+      <c r="P267" s="1">
+        <f t="shared" si="56"/>
+        <v>0.57002029615643346</v>
+      </c>
+      <c r="Q267" s="1">
+        <f t="shared" si="56"/>
+        <v>1.9434363731374738E-2</v>
+      </c>
+      <c r="R267" s="1">
+        <f t="shared" si="56"/>
+        <v>4.454760935528667E-3</v>
+      </c>
+      <c r="S267" s="1">
+        <f t="shared" si="56"/>
+        <v>0.10017871011141233</v>
+      </c>
+      <c r="T267" s="1">
+        <f t="shared" si="56"/>
+        <v>0.14060357246998162</v>
+      </c>
+      <c r="U267" s="1">
+        <f t="shared" si="56"/>
+        <v>8.6540154920590924E-3</v>
+      </c>
+    </row>
   </sheetData>
   <autoFilter ref="A1:K266" xr:uid="{00000000-0009-0000-0000-000001000000}">
     <sortState ref="A2:K266">
@@ -37719,7 +37798,19 @@
   <sortState ref="A2:V266">
     <sortCondition ref="A2"/>
   </sortState>
-  <conditionalFormatting sqref="M2:U266">
+  <conditionalFormatting sqref="M2:U267">
+    <cfRule type="colorScale" priority="20">
+      <colorScale>
+        <cfvo type="min"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="max"/>
+        <color rgb="FFF8696B"/>
+        <color rgb="FFFFEB84"/>
+        <color rgb="FF63BE7B"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="B2:B266">
     <cfRule type="colorScale" priority="19">
       <colorScale>
         <cfvo type="min"/>
@@ -37731,8 +37822,18 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="B2:B266">
+  <conditionalFormatting sqref="L2:L266">
     <cfRule type="colorScale" priority="18">
+      <colorScale>
+        <cfvo type="min"/>
+        <cfvo type="max"/>
+        <color rgb="FFFCFCFF"/>
+        <color rgb="FF63BE7B"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting pivot="1" sqref="Z4:AG4">
+    <cfRule type="colorScale" priority="4">
       <colorScale>
         <cfvo type="min"/>
         <cfvo type="percentile" val="50"/>
@@ -37743,17 +37844,7 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="L2:L266">
-    <cfRule type="colorScale" priority="17">
-      <colorScale>
-        <cfvo type="min"/>
-        <cfvo type="max"/>
-        <color rgb="FFFCFCFF"/>
-        <color rgb="FF63BE7B"/>
-      </colorScale>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting pivot="1" sqref="Z4:AG4">
+  <conditionalFormatting pivot="1" sqref="Z5:AG5">
     <cfRule type="colorScale" priority="3">
       <colorScale>
         <cfvo type="min"/>
@@ -37765,7 +37856,7 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting pivot="1" sqref="Z5:AG5">
+  <conditionalFormatting pivot="1" sqref="Z6:AG6">
     <cfRule type="colorScale" priority="2">
       <colorScale>
         <cfvo type="min"/>
@@ -37777,14 +37868,14 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting pivot="1" sqref="Z6:AG6">
+  <conditionalFormatting sqref="C267:K267">
     <cfRule type="colorScale" priority="1">
       <colorScale>
         <cfvo type="min"/>
         <cfvo type="percentile" val="50"/>
         <cfvo type="max"/>
         <color rgb="FFF8696B"/>
-        <color rgb="FFFFEB84"/>
+        <color rgb="FFFCFCFF"/>
         <color rgb="FF63BE7B"/>
       </colorScale>
     </cfRule>
@@ -37798,14 +37889,14 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{751DEEC3-F8CF-4F18-9D02-B44736607074}">
   <dimension ref="A1:Z266"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A85" workbookViewId="0">
-      <selection activeCell="X5" sqref="X5"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="E250" sqref="E250"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
     <col min="1" max="1" width="17.36328125" bestFit="1" customWidth="1"/>
-    <col min="2" max="10" width="0" hidden="1" customWidth="1"/>
+    <col min="2" max="10" width="8.7265625" customWidth="1"/>
     <col min="23" max="23" width="9.81640625" customWidth="1"/>
     <col min="24" max="24" width="22" bestFit="1" customWidth="1"/>
     <col min="25" max="25" width="12.36328125" bestFit="1" customWidth="1"/>
@@ -53303,47 +53394,47 @@
         <v>2</v>
       </c>
       <c r="K194">
-        <f t="shared" ref="K194:K257" si="36">SUM(B194:J194)</f>
+        <f t="shared" ref="K194:K240" si="36">SUM(B194:J194)</f>
         <v>252</v>
       </c>
       <c r="L194" s="1">
-        <f t="shared" ref="L194:L257" si="37">B194/K194</f>
+        <f t="shared" ref="L194:L240" si="37">B194/K194</f>
         <v>7.9365079365079361E-2</v>
       </c>
       <c r="M194" s="1">
-        <f t="shared" ref="M194:M257" si="38">C194/K194</f>
+        <f t="shared" ref="M194:M240" si="38">C194/K194</f>
         <v>3.1746031746031744E-2</v>
       </c>
       <c r="N194" s="1">
-        <f t="shared" ref="N194:N257" si="39">D194/K194</f>
+        <f t="shared" ref="N194:N240" si="39">D194/K194</f>
         <v>4.7619047619047616E-2</v>
       </c>
       <c r="O194" s="1">
-        <f t="shared" ref="O194:O257" si="40">E194/K194</f>
+        <f t="shared" ref="O194:O240" si="40">E194/K194</f>
         <v>0.31349206349206349</v>
       </c>
       <c r="P194" s="1">
-        <f t="shared" ref="P194:P257" si="41">F194/K194</f>
+        <f t="shared" ref="P194:P240" si="41">F194/K194</f>
         <v>0.15873015873015872</v>
       </c>
       <c r="Q194" s="1">
-        <f t="shared" ref="Q194:Q257" si="42">G194/K194</f>
+        <f t="shared" ref="Q194:Q240" si="42">G194/K194</f>
         <v>3.968253968253968E-3</v>
       </c>
       <c r="R194" s="1">
-        <f t="shared" ref="R194:R257" si="43">H194/K194</f>
+        <f t="shared" ref="R194:R240" si="43">H194/K194</f>
         <v>0.27777777777777779</v>
       </c>
       <c r="S194" s="1">
-        <f t="shared" ref="S194:S257" si="44">I194/K194</f>
+        <f t="shared" ref="S194:S240" si="44">I194/K194</f>
         <v>7.9365079365079361E-2</v>
       </c>
       <c r="T194" s="1">
-        <f t="shared" ref="T194:T257" si="45">J194/K194</f>
+        <f t="shared" ref="T194:T240" si="45">J194/K194</f>
         <v>7.9365079365079361E-3</v>
       </c>
       <c r="U194" s="5">
-        <f t="shared" ref="U194:U257" si="46">SUM(L194:T194)</f>
+        <f t="shared" ref="U194:U240" si="46">SUM(L194:T194)</f>
         <v>1</v>
       </c>
       <c r="W194" t="str">
@@ -57031,19 +57122,86 @@
         <v>%Protein</v>
       </c>
     </row>
-    <row r="241" spans="12:21" x14ac:dyDescent="0.35">
-      <c r="L241" s="1"/>
-      <c r="M241" s="1"/>
-      <c r="N241" s="1"/>
-      <c r="O241" s="1"/>
-      <c r="P241" s="1"/>
-      <c r="Q241" s="1"/>
-      <c r="R241" s="1"/>
-      <c r="S241" s="1"/>
-      <c r="T241" s="1"/>
+    <row r="241" spans="2:21" x14ac:dyDescent="0.35">
+      <c r="B241" s="9">
+        <f>SUM(B1:B240)</f>
+        <v>35263</v>
+      </c>
+      <c r="C241" s="9">
+        <f t="shared" ref="C241:K241" si="48">SUM(C1:C240)</f>
+        <v>12339</v>
+      </c>
+      <c r="D241" s="9">
+        <f t="shared" si="48"/>
+        <v>33171</v>
+      </c>
+      <c r="E241" s="9">
+        <f t="shared" si="48"/>
+        <v>133753</v>
+      </c>
+      <c r="F241" s="9">
+        <f t="shared" si="48"/>
+        <v>51533</v>
+      </c>
+      <c r="G241" s="9">
+        <f t="shared" si="48"/>
+        <v>5842</v>
+      </c>
+      <c r="H241" s="9">
+        <f t="shared" si="48"/>
+        <v>155140</v>
+      </c>
+      <c r="I241" s="9">
+        <f t="shared" si="48"/>
+        <v>27207</v>
+      </c>
+      <c r="J241" s="9">
+        <f t="shared" si="48"/>
+        <v>14614</v>
+      </c>
+      <c r="K241" s="9">
+        <f t="shared" si="48"/>
+        <v>468862</v>
+      </c>
+      <c r="L241" s="10">
+        <f>B241/$K$241</f>
+        <v>7.5209763213909417E-2</v>
+      </c>
+      <c r="M241" s="10">
+        <f t="shared" ref="M241:T241" si="49">C241/$K$241</f>
+        <v>2.6316912012489816E-2</v>
+      </c>
+      <c r="N241" s="10">
+        <f t="shared" si="49"/>
+        <v>7.0747895969389712E-2</v>
+      </c>
+      <c r="O241" s="10">
+        <f t="shared" si="49"/>
+        <v>0.28527157244562368</v>
+      </c>
+      <c r="P241" s="10">
+        <f t="shared" si="49"/>
+        <v>0.10991080531158422</v>
+      </c>
+      <c r="Q241" s="10">
+        <f t="shared" si="49"/>
+        <v>1.2459956234457047E-2</v>
+      </c>
+      <c r="R241" s="10">
+        <f t="shared" si="49"/>
+        <v>0.3308862735730343</v>
+      </c>
+      <c r="S241" s="10">
+        <f t="shared" si="49"/>
+        <v>5.802773523979337E-2</v>
+      </c>
+      <c r="T241" s="10">
+        <f t="shared" si="49"/>
+        <v>3.1169085999718467E-2</v>
+      </c>
       <c r="U241" s="5"/>
     </row>
-    <row r="242" spans="12:21" x14ac:dyDescent="0.35">
+    <row r="242" spans="2:21" x14ac:dyDescent="0.35">
       <c r="L242" s="1"/>
       <c r="M242" s="1"/>
       <c r="N242" s="1"/>
@@ -57055,7 +57213,7 @@
       <c r="T242" s="1"/>
       <c r="U242" s="5"/>
     </row>
-    <row r="243" spans="12:21" x14ac:dyDescent="0.35">
+    <row r="243" spans="2:21" x14ac:dyDescent="0.35">
       <c r="L243" s="1"/>
       <c r="M243" s="1"/>
       <c r="N243" s="1"/>
@@ -57067,7 +57225,7 @@
       <c r="T243" s="1"/>
       <c r="U243" s="5"/>
     </row>
-    <row r="244" spans="12:21" x14ac:dyDescent="0.35">
+    <row r="244" spans="2:21" x14ac:dyDescent="0.35">
       <c r="L244" s="1"/>
       <c r="M244" s="1"/>
       <c r="N244" s="1"/>
@@ -57079,7 +57237,7 @@
       <c r="T244" s="1"/>
       <c r="U244" s="5"/>
     </row>
-    <row r="245" spans="12:21" x14ac:dyDescent="0.35">
+    <row r="245" spans="2:21" x14ac:dyDescent="0.35">
       <c r="L245" s="1"/>
       <c r="M245" s="1"/>
       <c r="N245" s="1"/>
@@ -57091,7 +57249,7 @@
       <c r="T245" s="1"/>
       <c r="U245" s="5"/>
     </row>
-    <row r="246" spans="12:21" x14ac:dyDescent="0.35">
+    <row r="246" spans="2:21" x14ac:dyDescent="0.35">
       <c r="L246" s="1"/>
       <c r="M246" s="1"/>
       <c r="N246" s="1"/>
@@ -57103,7 +57261,7 @@
       <c r="T246" s="1"/>
       <c r="U246" s="5"/>
     </row>
-    <row r="247" spans="12:21" x14ac:dyDescent="0.35">
+    <row r="247" spans="2:21" x14ac:dyDescent="0.35">
       <c r="L247" s="1"/>
       <c r="M247" s="1"/>
       <c r="N247" s="1"/>
@@ -57115,7 +57273,7 @@
       <c r="T247" s="1"/>
       <c r="U247" s="5"/>
     </row>
-    <row r="248" spans="12:21" x14ac:dyDescent="0.35">
+    <row r="248" spans="2:21" x14ac:dyDescent="0.35">
       <c r="L248" s="1"/>
       <c r="M248" s="1"/>
       <c r="N248" s="1"/>
@@ -57127,7 +57285,7 @@
       <c r="T248" s="1"/>
       <c r="U248" s="5"/>
     </row>
-    <row r="249" spans="12:21" x14ac:dyDescent="0.35">
+    <row r="249" spans="2:21" x14ac:dyDescent="0.35">
       <c r="L249" s="1"/>
       <c r="M249" s="1"/>
       <c r="N249" s="1"/>
@@ -57139,7 +57297,7 @@
       <c r="T249" s="1"/>
       <c r="U249" s="5"/>
     </row>
-    <row r="250" spans="12:21" x14ac:dyDescent="0.35">
+    <row r="250" spans="2:21" x14ac:dyDescent="0.35">
       <c r="L250" s="1"/>
       <c r="M250" s="1"/>
       <c r="N250" s="1"/>
@@ -57151,7 +57309,7 @@
       <c r="T250" s="1"/>
       <c r="U250" s="5"/>
     </row>
-    <row r="251" spans="12:21" x14ac:dyDescent="0.35">
+    <row r="251" spans="2:21" x14ac:dyDescent="0.35">
       <c r="L251" s="1"/>
       <c r="M251" s="1"/>
       <c r="N251" s="1"/>
@@ -57163,7 +57321,7 @@
       <c r="T251" s="1"/>
       <c r="U251" s="5"/>
     </row>
-    <row r="252" spans="12:21" x14ac:dyDescent="0.35">
+    <row r="252" spans="2:21" x14ac:dyDescent="0.35">
       <c r="L252" s="1"/>
       <c r="M252" s="1"/>
       <c r="N252" s="1"/>
@@ -57175,7 +57333,7 @@
       <c r="T252" s="1"/>
       <c r="U252" s="5"/>
     </row>
-    <row r="253" spans="12:21" x14ac:dyDescent="0.35">
+    <row r="253" spans="2:21" x14ac:dyDescent="0.35">
       <c r="L253" s="1"/>
       <c r="M253" s="1"/>
       <c r="N253" s="1"/>
@@ -57187,7 +57345,7 @@
       <c r="T253" s="1"/>
       <c r="U253" s="5"/>
     </row>
-    <row r="254" spans="12:21" x14ac:dyDescent="0.35">
+    <row r="254" spans="2:21" x14ac:dyDescent="0.35">
       <c r="L254" s="1"/>
       <c r="M254" s="1"/>
       <c r="N254" s="1"/>
@@ -57199,7 +57357,7 @@
       <c r="T254" s="1"/>
       <c r="U254" s="5"/>
     </row>
-    <row r="255" spans="12:21" x14ac:dyDescent="0.35">
+    <row r="255" spans="2:21" x14ac:dyDescent="0.35">
       <c r="L255" s="1"/>
       <c r="M255" s="1"/>
       <c r="N255" s="1"/>
@@ -57211,7 +57369,7 @@
       <c r="T255" s="1"/>
       <c r="U255" s="5"/>
     </row>
-    <row r="256" spans="12:21" x14ac:dyDescent="0.35">
+    <row r="256" spans="2:21" x14ac:dyDescent="0.35">
       <c r="L256" s="1"/>
       <c r="M256" s="1"/>
       <c r="N256" s="1"/>
@@ -57346,7 +57504,7 @@
   </sheetData>
   <autoFilter ref="A1:AA240" xr:uid="{B5597D4A-4F76-46B6-A014-F1CAF2DEDC4C}"/>
   <conditionalFormatting sqref="L2:T266">
-    <cfRule type="colorScale" priority="6">
+    <cfRule type="colorScale" priority="7">
       <colorScale>
         <cfvo type="min"/>
         <cfvo type="percentile" val="50"/>
@@ -57357,8 +57515,8 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="K2:K266">
-    <cfRule type="colorScale" priority="4">
+  <conditionalFormatting sqref="K2:K240 K242:K266">
+    <cfRule type="colorScale" priority="5">
       <colorScale>
         <cfvo type="min"/>
         <cfvo type="max"/>
@@ -57367,7 +57525,20 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
+  <conditionalFormatting sqref="B241:J241">
+    <cfRule type="colorScale" priority="1">
+      <colorScale>
+        <cfvo type="min"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="max"/>
+        <color rgb="FFF8696B"/>
+        <color rgb="FFFCFCFF"/>
+        <color rgb="FF63BE7B"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <drawing r:id="rId2"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId2"/>
+  <drawing r:id="rId3"/>
 </worksheet>
 </file>
</xml_diff>